<commit_message>
feat: add matrix of the graphs
</commit_message>
<xml_diff>
--- a/assets/matrixs/fourmillere_zero.xlsx
+++ b/assets/matrixs/fourmillere_zero.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projets_GIT\uneviedefourmi\assets\matrixs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41793F4D-B4C9-4F0A-9739-A8BAE92E71DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D5C31A-573E-4FA2-9789-247EDB511050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrice d'adjacence" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
+  <si>
+    <t>Vestibule</t>
+  </si>
+  <si>
+    <t>Dortoir</t>
+  </si>
+  <si>
+    <t>Salle 1</t>
+  </si>
+  <si>
+    <t>Salle 2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45,7 +62,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -53,12 +70,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,36 +466,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="A1:G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8347BA9-335B-43BF-900A-FB06D5589A2B}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87447CA-7B48-4DB1-8A93-081BA0E7270E}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>